<commit_message>
0.6.1 - Tasks Import upgraded and fully correct and working
</commit_message>
<xml_diff>
--- a/keel_task_import_template.xlsx
+++ b/keel_task_import_template.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E986B6EE-8697-4842-AD04-12453C63F924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="_meta" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet sheetId="1" name="Tasks" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="_meta" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>part_number</t>
   </si>
@@ -42,13 +38,31 @@
     <t>department</t>
   </si>
   <si>
+    <t>trainee_type</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>safety_requirements</t>
+  </si>
+  <si>
+    <t>evidence_type</t>
+  </si>
+  <si>
+    <t>verification_method</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
     <t>Navigation</t>
   </si>
   <si>
-    <t>Determine position using terrestrial observations</t>
-  </si>
-  <si>
-    <t>Use cross bearings to fix position on chart.</t>
+    <t>Visual Bearings</t>
+  </si>
+  <si>
+    <t>Use azimuth circle</t>
   </si>
   <si>
     <t>A-II/1</t>
@@ -61,6 +75,24 @@
   </si>
   <si>
     <t>Deck</t>
+  </si>
+  <si>
+    <t>DECK_CADET</t>
+  </si>
+  <si>
+    <t>Standard bridge procedure.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>PHOTO</t>
+  </si>
+  <si>
+    <t>OBSERVATION</t>
+  </si>
+  <si>
+    <t>ONCE</t>
   </si>
   <si>
     <t>Bulk Carrier</t>
@@ -105,14 +137,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -475,25 +507,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1000"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
+    <col min="11" max="11" width="30" customWidth="1"/>
+    <col min="12" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,131 +550,1183 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
       </c>
     </row>
+    <row r="3" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="257" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="258" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="259" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="260" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="261" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="263" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="264" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="265" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="275" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="276" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="277" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="278" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="301" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="302" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="303" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="304" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="305" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="306" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="307" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="308" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="309" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="310" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="311" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="312" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="313" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="314" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="315" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="316" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="317" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="318" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="319" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="320" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="321" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="322" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="323" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="324" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="325" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="326" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="327" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="328" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="329" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="330" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="331" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="332" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="333" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="334" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="335" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="336" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="337" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="338" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="339" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="340" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="341" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="342" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="343" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="344" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="345" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="346" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="347" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="348" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="349" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="350" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="351" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="352" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="353" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="354" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="355" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="356" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="357" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="358" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="359" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="360" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="361" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="362" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="363" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="364" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="365" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="366" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="367" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="368" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="369" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="370" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="371" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="372" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="373" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="374" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="375" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="376" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="377" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="378" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="379" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="380" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="381" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="382" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="383" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="384" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="385" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="386" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="387" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="388" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="389" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="390" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="391" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="392" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="393" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="394" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="395" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="396" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="397" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="398" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="399" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="400" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="401" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="402" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="403" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="404" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="405" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="406" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="407" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="408" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="409" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="410" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="411" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="412" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="413" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="414" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="415" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="416" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="417" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="418" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="419" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="420" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="421" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="422" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="423" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="424" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="425" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="426" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="427" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="428" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="429" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="430" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="431" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="432" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="433" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="434" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="435" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="436" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="437" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="438" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="439" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="440" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="441" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="442" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="443" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="444" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="445" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="446" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="447" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="448" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="449" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="450" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="451" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="452" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="453" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="454" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="455" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="456" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="457" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="458" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="459" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="460" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="461" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="462" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="463" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="464" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="465" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="466" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="467" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="468" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="469" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="470" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="471" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="472" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="473" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="474" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="475" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="476" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="477" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="478" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="479" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="480" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="481" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="482" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="483" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="484" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="485" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="486" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="487" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="488" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="489" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="490" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="491" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="492" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="493" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="494" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="495" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="496" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="497" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="498" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="499" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="500" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="501" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="502" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="503" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="504" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="505" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="506" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="507" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="508" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="509" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="510" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="511" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="512" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="513" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="514" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="515" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="516" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="517" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="518" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="519" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="520" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="521" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="522" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="523" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="524" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="525" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="526" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="527" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="528" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="529" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="530" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="531" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="532" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="533" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="534" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="535" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="536" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="537" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="538" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="539" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="540" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="541" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="542" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="543" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="544" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="545" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="546" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="547" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="548" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="549" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="550" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="551" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="552" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="553" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="554" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="555" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="556" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="557" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="558" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="559" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="560" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="561" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="562" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="563" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="564" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="565" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="566" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="567" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="568" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="569" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="570" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="571" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="572" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="573" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="574" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="575" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="576" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="577" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="578" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="579" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="580" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="581" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="582" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="583" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="584" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="585" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="586" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="587" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="588" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="589" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="590" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="591" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="592" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="593" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="594" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="595" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="596" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="597" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="598" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="599" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="600" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="601" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="602" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="603" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="604" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="605" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="606" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="607" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="608" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="609" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="610" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="611" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="612" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="613" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="614" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="615" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="616" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="617" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="618" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="619" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="620" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="621" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="622" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="623" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="624" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="625" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="626" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="627" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="628" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="629" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="630" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="631" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="632" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="633" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="634" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="635" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="636" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="637" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="638" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="639" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="640" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="641" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="642" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="643" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="644" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="645" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="646" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="647" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="648" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="649" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="650" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="651" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="652" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="653" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="654" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="655" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="656" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="657" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="658" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="659" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="660" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="661" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="662" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="663" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="664" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="665" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="666" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="667" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="668" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="669" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="670" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="671" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="672" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="673" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="674" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="675" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="676" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="677" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="678" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="679" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="680" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="681" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="682" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="683" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="684" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="685" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="686" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="687" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="688" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="689" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="690" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="691" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="692" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="693" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="694" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="695" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="696" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="697" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="698" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="699" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="700" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="701" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="702" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="703" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="704" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="705" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="706" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="707" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="708" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="709" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="710" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="711" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="712" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="713" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="714" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="715" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="716" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="717" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="718" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="719" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="720" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="721" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="722" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="723" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="724" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="725" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="726" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="727" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="728" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="729" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="730" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="731" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="732" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="733" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="734" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="735" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="736" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="737" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="738" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="739" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="740" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="741" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="742" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="743" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="744" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="745" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="746" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="747" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="748" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="749" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="750" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="751" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="752" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="753" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="754" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="755" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="756" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="757" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="758" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="759" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="760" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="761" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="762" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="763" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="764" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="765" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="766" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="767" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="768" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="769" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="770" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="771" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="772" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="773" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="774" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="775" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="776" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="777" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="778" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="779" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="780" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="781" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="782" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="783" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="784" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="785" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="786" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="787" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="788" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="789" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="790" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="791" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="792" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="793" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="794" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="795" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="796" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="797" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="798" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="799" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="800" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="801" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="802" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="803" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="804" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="805" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="806" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="807" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="808" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="809" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="810" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="811" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="812" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="813" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="814" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="815" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="816" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="817" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="818" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="819" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="820" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="821" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="822" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="823" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="824" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="825" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="826" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="827" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="828" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="829" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="830" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="831" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="832" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="833" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="834" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="835" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="836" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="837" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="838" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="839" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="840" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="841" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="842" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="843" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="844" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="845" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="846" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="847" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="848" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="849" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="850" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="851" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="852" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="853" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="854" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="855" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="856" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="857" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="858" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="859" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="860" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="861" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="862" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="863" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="864" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="865" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="866" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="867" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="868" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="869" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="870" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="871" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="872" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="873" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="874" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="875" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="876" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="877" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="878" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="879" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="880" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="881" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="882" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="883" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="884" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="885" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="886" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="887" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="888" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="889" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="890" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="891" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="892" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="893" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="894" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="895" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="896" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="897" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="898" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="899" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="900" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="901" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="902" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="903" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="904" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="905" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="906" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="907" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="908" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="909" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="910" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="911" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="912" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="913" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="914" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="915" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="916" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="917" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="918" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="919" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="920" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="921" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="922" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="923" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="924" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="925" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="926" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="927" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="928" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="929" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="930" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="931" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="932" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="933" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="934" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="935" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="936" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="937" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="938" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="939" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="940" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="941" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="942" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="943" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="944" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="945" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="946" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="947" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="948" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="949" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="950" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="951" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="952" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="953" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="954" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="955" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="956" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="957" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="958" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="959" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="960" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="961" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="962" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="963" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="964" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="965" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="966" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="967" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="968" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="969" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="970" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="971" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="972" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="973" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="974" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="975" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="976" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="977" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="978" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="979" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="980" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="981" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="982" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="983" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="984" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="985" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="986" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="987" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="988" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="989" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="990" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="991" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="992" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="993" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="994" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="995" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="996" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="997" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="998" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="999" spans="7:14" x14ac:dyDescent="0.25"/>
+    <row r="1000" spans="7:14" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Department" error="Please select from: Deck, Engine, Electrical, Catering, General" sqref="H2:H1000" xr:uid="{00000000-0002-0000-0000-000002000000}">
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" sqref="G10:G1000">
+      <formula1>_meta!$A$1:$A$13</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="G2:G1000">
+      <formula1>_meta!$A$1:$A$13</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="H10:H1000">
       <formula1>"Deck,Engine,Electrical,Catering,General"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="H2:H1000">
+      <formula1>"Deck,Engine,Electrical,Catering,General"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showErrorMessage="1" errorTitle="Invalid Trainee Type" error="Must be: DECK_CADET, ENGINE_CADET, ETO_CADET, DECK_RATING, or ENGINE_RATING" sqref="I10:I1000">
+      <formula1>"DECK_CADET,ENGINE_CADET,ETO_CADET,DECK_RATING,ENGINE_RATING"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showErrorMessage="1" errorTitle="Invalid Trainee Type" error="Must be: DECK_CADET, ENGINE_CADET, ETO_CADET, DECK_RATING, or ENGINE_RATING" sqref="I2:I1000">
+      <formula1>"DECK_CADET,ENGINE_CADET,ETO_CADET,DECK_RATING,ENGINE_RATING"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="L10:L1000">
+      <formula1>"PHOTO,VIDEO,DOCUMENT,NONE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="L2:L1000">
+      <formula1>"PHOTO,VIDEO,DOCUMENT,NONE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="M10:M1000">
+      <formula1>"OBSERVATION,Q&amp;A,SIMULATION,CHECKLIST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="M2:M1000">
+      <formula1>"OBSERVATION,Q&amp;A,SIMULATION,CHECKLIST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="N10:N1000">
+      <formula1>"ONCE,MONTHLY,QUARTERLY"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="N2:N1000">
+      <formula1>"ONCE,MONTHLY,QUARTERLY"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Ship Type" error="Select a valid Ship Type or leave blank for Universal." xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>_meta!$A$1:$A$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1000</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
0.8.1 - Updated Tree.
</commit_message>
<xml_diff>
--- a/keel_task_import_template.xlsx
+++ b/keel_task_import_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98C49F5-DE7B-4931-9F9E-7FA80F36CE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD1A802-5974-4651-83E9-51F5A5C4CF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6644,7 +6644,7 @@
   <dimension ref="A1:N938"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>